<commit_message>
tests - 97% line coverage
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanjanku_1/Downloads/Excel to SQL Converter/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DE6400-52BA-1C41-9ECC-0BDB70B41C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D943746-6F90-AC48-A166-472C675EC2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="99">
   <si>
     <t>HashiCorp Certified: Terraform Associate (003)</t>
   </si>
@@ -325,9 +325,6 @@
     <t>1 Year</t>
   </si>
   <si>
-    <t>po</t>
-  </si>
-  <si>
     <t>name*</t>
   </si>
   <si>
@@ -341,9 +338,6 @@
   </si>
   <si>
     <t>status&gt;Aktive=ACTIVE&amp;?=INACTIVE</t>
-  </si>
-  <si>
-    <t>Jo</t>
   </si>
   <si>
     <t>transcript&gt;Po=true&amp;Jo=false</t>
@@ -957,9 +951,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31:J197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -980,34 +974,34 @@
   <sheetData>
     <row r="1" spans="1:31" ht="16">
       <c r="A1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="6"/>
@@ -2470,9 +2464,7 @@
       <c r="G31" s="29"/>
       <c r="H31" s="35"/>
       <c r="I31" s="29"/>
-      <c r="J31" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J31" s="3"/>
       <c r="K31" s="1"/>
       <c r="L31" s="10"/>
       <c r="M31" s="1"/>
@@ -2505,9 +2497,7 @@
       <c r="G32" s="29"/>
       <c r="H32" s="35"/>
       <c r="I32" s="29"/>
-      <c r="J32" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J32" s="3"/>
       <c r="K32" s="1"/>
       <c r="L32" s="10"/>
       <c r="M32" s="1"/>
@@ -2672,9 +2662,7 @@
       <c r="G37" s="29"/>
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
-      <c r="J37" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J37" s="3"/>
       <c r="K37" s="1"/>
       <c r="L37" s="10"/>
       <c r="M37" s="1"/>
@@ -2707,9 +2695,7 @@
       <c r="G38" s="29"/>
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
-      <c r="J38" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="1"/>
       <c r="L38" s="10"/>
       <c r="M38" s="1"/>
@@ -2742,9 +2728,7 @@
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
-      <c r="J39" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="1"/>
       <c r="L39" s="10"/>
       <c r="M39" s="1"/>
@@ -2777,9 +2761,7 @@
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
       <c r="I40" s="29"/>
-      <c r="J40" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J40" s="3"/>
       <c r="K40" s="1"/>
       <c r="L40" s="10"/>
       <c r="M40" s="1"/>
@@ -2878,9 +2860,7 @@
       <c r="G43" s="29"/>
       <c r="H43" s="29"/>
       <c r="I43" s="29"/>
-      <c r="J43" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J43" s="3"/>
       <c r="K43" s="1"/>
       <c r="L43" s="10"/>
       <c r="M43" s="1"/>
@@ -2979,9 +2959,7 @@
       <c r="G46" s="29"/>
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
-      <c r="J46" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J46" s="3"/>
       <c r="K46" s="1"/>
       <c r="L46" s="10"/>
       <c r="M46" s="1"/>
@@ -3113,9 +3091,7 @@
       <c r="G50" s="29"/>
       <c r="H50" s="29"/>
       <c r="I50" s="29"/>
-      <c r="J50" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J50" s="3"/>
       <c r="K50" s="1"/>
       <c r="L50" s="10"/>
       <c r="M50" s="1"/>
@@ -3313,9 +3289,7 @@
       <c r="G56" s="29"/>
       <c r="H56" s="29"/>
       <c r="I56" s="29"/>
-      <c r="J56" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J56" s="3"/>
       <c r="K56" s="1"/>
       <c r="L56" s="10"/>
       <c r="M56" s="1"/>
@@ -3348,9 +3322,7 @@
       <c r="G57" s="29"/>
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
-      <c r="J57" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J57" s="3"/>
       <c r="K57" s="1"/>
       <c r="L57" s="10"/>
       <c r="M57" s="1"/>
@@ -3383,9 +3355,7 @@
       <c r="G58" s="29"/>
       <c r="H58" s="29"/>
       <c r="I58" s="29"/>
-      <c r="J58" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J58" s="3"/>
       <c r="K58" s="1"/>
       <c r="L58" s="10"/>
       <c r="M58" s="1"/>
@@ -3418,9 +3388,7 @@
       <c r="G59" s="29"/>
       <c r="H59" s="29"/>
       <c r="I59" s="29"/>
-      <c r="J59" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J59" s="3"/>
       <c r="K59" s="1"/>
       <c r="L59" s="10"/>
       <c r="M59" s="1"/>
@@ -3453,9 +3421,7 @@
       <c r="G60" s="29"/>
       <c r="H60" s="29"/>
       <c r="I60" s="29"/>
-      <c r="J60" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J60" s="3"/>
       <c r="K60" s="1"/>
       <c r="L60" s="10"/>
       <c r="M60" s="1"/>
@@ -3488,9 +3454,7 @@
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
       <c r="I61" s="29"/>
-      <c r="J61" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J61" s="3"/>
       <c r="K61" s="1"/>
       <c r="L61" s="10"/>
       <c r="M61" s="1"/>
@@ -3556,9 +3520,7 @@
       <c r="G63" s="29"/>
       <c r="H63" s="29"/>
       <c r="I63" s="29"/>
-      <c r="J63" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J63" s="3"/>
       <c r="K63" s="1"/>
       <c r="L63" s="10"/>
       <c r="M63" s="1"/>
@@ -3591,9 +3553,7 @@
       <c r="G64" s="29"/>
       <c r="H64" s="29"/>
       <c r="I64" s="29"/>
-      <c r="J64" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J64" s="3"/>
       <c r="K64" s="1"/>
       <c r="L64" s="10"/>
       <c r="M64" s="1"/>
@@ -3659,9 +3619,7 @@
       <c r="G66" s="29"/>
       <c r="H66" s="29"/>
       <c r="I66" s="29"/>
-      <c r="J66" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J66" s="3"/>
       <c r="K66" s="1"/>
       <c r="L66" s="10"/>
       <c r="M66" s="1"/>
@@ -3694,9 +3652,7 @@
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
       <c r="I67" s="29"/>
-      <c r="J67" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J67" s="3"/>
       <c r="K67" s="1"/>
       <c r="L67" s="10"/>
       <c r="M67" s="1"/>
@@ -3729,9 +3685,7 @@
       <c r="G68" s="29"/>
       <c r="H68" s="29"/>
       <c r="I68" s="29"/>
-      <c r="J68" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J68" s="3"/>
       <c r="K68" s="1"/>
       <c r="L68" s="10"/>
       <c r="M68" s="1"/>
@@ -3764,9 +3718,7 @@
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
-      <c r="J69" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J69" s="3"/>
       <c r="K69" s="1"/>
       <c r="L69" s="10"/>
       <c r="M69" s="1"/>
@@ -3799,9 +3751,7 @@
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
       <c r="I70" s="29"/>
-      <c r="J70" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J70" s="3"/>
       <c r="K70" s="1"/>
       <c r="L70" s="10"/>
       <c r="M70" s="1"/>
@@ -3900,9 +3850,7 @@
       <c r="G73" s="29"/>
       <c r="H73" s="29"/>
       <c r="I73" s="29"/>
-      <c r="J73" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J73" s="3"/>
       <c r="K73" s="1"/>
       <c r="L73" s="10"/>
       <c r="M73" s="1"/>
@@ -3935,9 +3883,7 @@
       <c r="G74" s="29"/>
       <c r="H74" s="29"/>
       <c r="I74" s="29"/>
-      <c r="J74" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J74" s="3"/>
       <c r="K74" s="1"/>
       <c r="L74" s="10"/>
       <c r="M74" s="1"/>
@@ -3970,9 +3916,7 @@
       <c r="G75" s="29"/>
       <c r="H75" s="29"/>
       <c r="I75" s="29"/>
-      <c r="J75" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J75" s="3"/>
       <c r="K75" s="1"/>
       <c r="L75" s="10"/>
       <c r="M75" s="1"/>
@@ -4038,9 +3982,7 @@
       <c r="G77" s="29"/>
       <c r="H77" s="29"/>
       <c r="I77" s="29"/>
-      <c r="J77" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J77" s="3"/>
       <c r="K77" s="1"/>
       <c r="L77" s="10"/>
       <c r="M77" s="1"/>
@@ -4073,9 +4015,7 @@
       <c r="G78" s="29"/>
       <c r="H78" s="29"/>
       <c r="I78" s="29"/>
-      <c r="J78" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J78" s="3"/>
       <c r="K78" s="1"/>
       <c r="L78" s="10"/>
       <c r="M78" s="1"/>
@@ -4108,9 +4048,7 @@
       <c r="G79" s="29"/>
       <c r="H79" s="29"/>
       <c r="I79" s="29"/>
-      <c r="J79" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J79" s="3"/>
       <c r="K79" s="1"/>
       <c r="L79" s="10"/>
       <c r="M79" s="1"/>
@@ -4143,9 +4081,7 @@
       <c r="G80" s="29"/>
       <c r="H80" s="29"/>
       <c r="I80" s="29"/>
-      <c r="J80" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J80" s="3"/>
       <c r="K80" s="1"/>
       <c r="L80" s="10"/>
       <c r="M80" s="1"/>
@@ -4178,9 +4114,7 @@
       <c r="G81" s="29"/>
       <c r="H81" s="29"/>
       <c r="I81" s="29"/>
-      <c r="J81" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J81" s="3"/>
       <c r="K81" s="1"/>
       <c r="L81" s="10"/>
       <c r="M81" s="1"/>
@@ -4213,9 +4147,7 @@
       <c r="G82" s="29"/>
       <c r="H82" s="29"/>
       <c r="I82" s="29"/>
-      <c r="J82" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J82" s="3"/>
       <c r="K82" s="1"/>
       <c r="L82" s="10"/>
       <c r="M82" s="1"/>
@@ -4248,9 +4180,7 @@
       <c r="G83" s="29"/>
       <c r="H83" s="29"/>
       <c r="I83" s="29"/>
-      <c r="J83" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J83" s="3"/>
       <c r="K83" s="1"/>
       <c r="L83" s="10"/>
       <c r="M83" s="1"/>
@@ -4283,9 +4213,7 @@
       <c r="G84" s="29"/>
       <c r="H84" s="29"/>
       <c r="I84" s="29"/>
-      <c r="J84" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J84" s="3"/>
       <c r="K84" s="1"/>
       <c r="L84" s="10"/>
       <c r="M84" s="1"/>
@@ -4318,9 +4246,7 @@
       <c r="G85" s="29"/>
       <c r="H85" s="29"/>
       <c r="I85" s="29"/>
-      <c r="J85" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J85" s="3"/>
       <c r="K85" s="1"/>
       <c r="L85" s="10"/>
       <c r="M85" s="1"/>
@@ -4353,9 +4279,7 @@
       <c r="G86" s="29"/>
       <c r="H86" s="29"/>
       <c r="I86" s="29"/>
-      <c r="J86" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J86" s="3"/>
       <c r="K86" s="1"/>
       <c r="L86" s="10"/>
       <c r="M86" s="1"/>
@@ -4388,9 +4312,7 @@
       <c r="G87" s="29"/>
       <c r="H87" s="29"/>
       <c r="I87" s="29"/>
-      <c r="J87" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J87" s="3"/>
       <c r="K87" s="1"/>
       <c r="L87" s="10"/>
       <c r="M87" s="1"/>
@@ -4423,9 +4345,7 @@
       <c r="G88" s="29"/>
       <c r="H88" s="29"/>
       <c r="I88" s="29"/>
-      <c r="J88" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J88" s="3"/>
       <c r="K88" s="1"/>
       <c r="L88" s="10"/>
       <c r="M88" s="1"/>
@@ -4458,9 +4378,7 @@
       <c r="G89" s="29"/>
       <c r="H89" s="29"/>
       <c r="I89" s="29"/>
-      <c r="J89" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J89" s="3"/>
       <c r="K89" s="1"/>
       <c r="L89" s="10"/>
       <c r="M89" s="1"/>
@@ -4493,9 +4411,7 @@
       <c r="G90" s="29"/>
       <c r="H90" s="29"/>
       <c r="I90" s="29"/>
-      <c r="J90" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J90" s="3"/>
       <c r="K90" s="1"/>
       <c r="L90" s="10"/>
       <c r="M90" s="1"/>
@@ -4528,9 +4444,7 @@
       <c r="G91" s="29"/>
       <c r="H91" s="35"/>
       <c r="I91" s="29"/>
-      <c r="J91" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J91" s="3"/>
       <c r="K91" s="1"/>
       <c r="L91" s="24"/>
       <c r="M91" s="1"/>
@@ -4728,9 +4642,7 @@
       <c r="G97" s="29"/>
       <c r="H97" s="29"/>
       <c r="I97" s="29"/>
-      <c r="J97" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J97" s="3"/>
       <c r="K97" s="1"/>
       <c r="L97" s="10"/>
       <c r="M97" s="1"/>
@@ -4763,9 +4675,7 @@
       <c r="G98" s="29"/>
       <c r="H98" s="35"/>
       <c r="I98" s="29"/>
-      <c r="J98" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J98" s="3"/>
       <c r="K98" s="1"/>
       <c r="L98" s="10"/>
       <c r="M98" s="1"/>
@@ -4798,9 +4708,7 @@
       <c r="G99" s="29"/>
       <c r="H99" s="35"/>
       <c r="I99" s="29"/>
-      <c r="J99" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J99" s="3"/>
       <c r="K99" s="1"/>
       <c r="L99" s="10"/>
       <c r="M99" s="1"/>
@@ -4899,9 +4807,7 @@
       <c r="G102" s="29"/>
       <c r="H102" s="35"/>
       <c r="I102" s="29"/>
-      <c r="J102" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J102" s="3"/>
       <c r="K102" s="1"/>
       <c r="L102" s="10"/>
       <c r="M102" s="1"/>
@@ -5264,9 +5170,7 @@
       <c r="G113" s="29"/>
       <c r="H113" s="29"/>
       <c r="I113" s="29"/>
-      <c r="J113" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J113" s="3"/>
       <c r="K113" s="1"/>
       <c r="L113" s="10"/>
       <c r="M113" s="1"/>
@@ -5332,9 +5236,7 @@
       <c r="G115" s="29"/>
       <c r="H115" s="35"/>
       <c r="I115" s="29"/>
-      <c r="J115" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J115" s="3"/>
       <c r="K115" s="1"/>
       <c r="L115" s="10"/>
       <c r="M115" s="1"/>
@@ -5367,9 +5269,7 @@
       <c r="G116" s="29"/>
       <c r="H116" s="29"/>
       <c r="I116" s="29"/>
-      <c r="J116" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J116" s="3"/>
       <c r="K116" s="1"/>
       <c r="L116" s="10"/>
       <c r="M116" s="1"/>
@@ -5402,9 +5302,7 @@
       <c r="G117" s="29"/>
       <c r="H117" s="29"/>
       <c r="I117" s="29"/>
-      <c r="J117" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J117" s="3"/>
       <c r="K117" s="1"/>
       <c r="L117" s="10"/>
       <c r="M117" s="1"/>
@@ -5437,9 +5335,7 @@
       <c r="G118" s="29"/>
       <c r="H118" s="35"/>
       <c r="I118" s="29"/>
-      <c r="J118" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J118" s="3"/>
       <c r="K118" s="1"/>
       <c r="L118" s="26"/>
       <c r="M118" s="1"/>
@@ -5472,9 +5368,7 @@
       <c r="G119" s="29"/>
       <c r="H119" s="29"/>
       <c r="I119" s="29"/>
-      <c r="J119" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J119" s="3"/>
       <c r="K119" s="1"/>
       <c r="L119" s="10"/>
       <c r="M119" s="1"/>
@@ -5606,9 +5500,7 @@
       <c r="G123" s="29"/>
       <c r="H123" s="29"/>
       <c r="I123" s="29"/>
-      <c r="J123" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J123" s="3"/>
       <c r="K123" s="1"/>
       <c r="L123" s="10"/>
       <c r="M123" s="1"/>
@@ -5641,9 +5533,7 @@
       <c r="G124" s="29"/>
       <c r="H124" s="29"/>
       <c r="I124" s="29"/>
-      <c r="J124" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J124" s="3"/>
       <c r="K124" s="1"/>
       <c r="L124" s="10"/>
       <c r="M124" s="1"/>
@@ -5676,9 +5566,7 @@
       <c r="G125" s="29"/>
       <c r="H125" s="35"/>
       <c r="I125" s="29"/>
-      <c r="J125" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="J125" s="3"/>
       <c r="K125" s="1"/>
       <c r="L125" s="10"/>
       <c r="M125" s="1"/>
@@ -5711,9 +5599,7 @@
       <c r="G126" s="29"/>
       <c r="H126" s="29"/>
       <c r="I126" s="29"/>
-      <c r="J126" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J126" s="3"/>
       <c r="K126" s="1"/>
       <c r="L126" s="10"/>
       <c r="M126" s="1"/>
@@ -5779,9 +5665,7 @@
       <c r="G128" s="29"/>
       <c r="H128" s="29"/>
       <c r="I128" s="29"/>
-      <c r="J128" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J128" s="3"/>
       <c r="K128" s="1"/>
       <c r="L128" s="10"/>
       <c r="M128" s="1"/>
@@ -5814,9 +5698,7 @@
       <c r="G129" s="29"/>
       <c r="H129" s="29"/>
       <c r="I129" s="29"/>
-      <c r="J129" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J129" s="3"/>
       <c r="K129" s="1"/>
       <c r="L129" s="10"/>
       <c r="M129" s="1"/>
@@ -5849,9 +5731,7 @@
       <c r="G130" s="29"/>
       <c r="H130" s="29"/>
       <c r="I130" s="29"/>
-      <c r="J130" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J130" s="3"/>
       <c r="K130" s="1"/>
       <c r="L130" s="10"/>
       <c r="M130" s="1"/>
@@ -5917,9 +5797,7 @@
       <c r="G132" s="29"/>
       <c r="H132" s="29"/>
       <c r="I132" s="29"/>
-      <c r="J132" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J132" s="3"/>
       <c r="K132" s="1"/>
       <c r="L132" s="10"/>
       <c r="M132" s="1"/>
@@ -5985,9 +5863,7 @@
       <c r="G134" s="29"/>
       <c r="H134" s="29"/>
       <c r="I134" s="29"/>
-      <c r="J134" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J134" s="3"/>
       <c r="K134" s="1"/>
       <c r="L134" s="10"/>
       <c r="M134" s="1"/>
@@ -6020,9 +5896,7 @@
       <c r="G135" s="29"/>
       <c r="H135" s="29"/>
       <c r="I135" s="29"/>
-      <c r="J135" s="3" t="s">
-        <v>95</v>
-      </c>
+      <c r="J135" s="3"/>
       <c r="K135" s="1"/>
       <c r="L135" s="10"/>
       <c r="M135" s="1"/>
@@ -6154,9 +6028,7 @@
       <c r="G139" s="29"/>
       <c r="H139" s="29"/>
       <c r="I139" s="29"/>
-      <c r="J139" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J139" s="3"/>
       <c r="K139" s="1"/>
       <c r="L139" s="10"/>
       <c r="M139" s="1"/>
@@ -6189,9 +6061,7 @@
       <c r="G140" s="29"/>
       <c r="H140" s="29"/>
       <c r="I140" s="29"/>
-      <c r="J140" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J140" s="3"/>
       <c r="K140" s="1"/>
       <c r="L140" s="10"/>
       <c r="M140" s="1"/>
@@ -6257,9 +6127,7 @@
       <c r="G142" s="29"/>
       <c r="H142" s="29"/>
       <c r="I142" s="29"/>
-      <c r="J142" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J142" s="3"/>
       <c r="K142" s="1"/>
       <c r="L142" s="10"/>
       <c r="M142" s="1"/>
@@ -6292,9 +6160,7 @@
       <c r="G143" s="29"/>
       <c r="H143" s="35"/>
       <c r="I143" s="29"/>
-      <c r="J143" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J143" s="3"/>
       <c r="K143" s="1"/>
       <c r="L143" s="25"/>
       <c r="M143" s="1"/>
@@ -6327,9 +6193,7 @@
       <c r="G144" s="29"/>
       <c r="H144" s="35"/>
       <c r="I144" s="29"/>
-      <c r="J144" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J144" s="3"/>
       <c r="K144" s="1"/>
       <c r="L144" s="10"/>
       <c r="M144" s="1"/>
@@ -6362,9 +6226,7 @@
       <c r="G145" s="29"/>
       <c r="H145" s="35"/>
       <c r="I145" s="29"/>
-      <c r="J145" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J145" s="3"/>
       <c r="K145" s="1"/>
       <c r="L145" s="27"/>
       <c r="M145" s="1"/>
@@ -6463,9 +6325,7 @@
       <c r="G148" s="29"/>
       <c r="H148" s="29"/>
       <c r="I148" s="29"/>
-      <c r="J148" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J148" s="3"/>
       <c r="K148" s="1"/>
       <c r="L148" s="10"/>
       <c r="M148" s="1"/>
@@ -6531,9 +6391,7 @@
       <c r="G150" s="29"/>
       <c r="H150" s="29"/>
       <c r="I150" s="29"/>
-      <c r="J150" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J150" s="3"/>
       <c r="K150" s="1"/>
       <c r="L150" s="10"/>
       <c r="M150" s="1"/>
@@ -6632,9 +6490,7 @@
       <c r="G153" s="29"/>
       <c r="H153" s="35"/>
       <c r="I153" s="29"/>
-      <c r="J153" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J153" s="3"/>
       <c r="K153" s="1"/>
       <c r="L153" s="10"/>
       <c r="M153" s="1"/>
@@ -6667,9 +6523,7 @@
       <c r="G154" s="29"/>
       <c r="H154" s="29"/>
       <c r="I154" s="29"/>
-      <c r="J154" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J154" s="3"/>
       <c r="K154" s="1"/>
       <c r="L154" s="10"/>
       <c r="M154" s="1"/>
@@ -6702,9 +6556,7 @@
       <c r="G155" s="29"/>
       <c r="H155" s="29"/>
       <c r="I155" s="29"/>
-      <c r="J155" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J155" s="3"/>
       <c r="K155" s="1"/>
       <c r="L155" s="24"/>
       <c r="M155" s="1"/>
@@ -6737,9 +6589,7 @@
       <c r="G156" s="29"/>
       <c r="H156" s="29"/>
       <c r="I156" s="29"/>
-      <c r="J156" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J156" s="3"/>
       <c r="K156" s="1"/>
       <c r="L156" s="24"/>
       <c r="M156" s="1"/>
@@ -6772,9 +6622,7 @@
       <c r="G157" s="29"/>
       <c r="H157" s="29"/>
       <c r="I157" s="29"/>
-      <c r="J157" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J157" s="3"/>
       <c r="K157" s="1"/>
       <c r="L157" s="24"/>
       <c r="M157" s="1"/>
@@ -6939,9 +6787,7 @@
       <c r="G162" s="29"/>
       <c r="H162" s="29"/>
       <c r="I162" s="29"/>
-      <c r="J162" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J162" s="3"/>
       <c r="K162" s="1"/>
       <c r="L162" s="10"/>
       <c r="M162" s="1"/>
@@ -7040,9 +6886,7 @@
       <c r="G165" s="29"/>
       <c r="H165" s="29"/>
       <c r="I165" s="29"/>
-      <c r="J165" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J165" s="3"/>
       <c r="K165" s="1"/>
       <c r="L165" s="10"/>
       <c r="M165" s="1"/>
@@ -7075,9 +6919,7 @@
       <c r="G166" s="29"/>
       <c r="H166" s="35"/>
       <c r="I166" s="29"/>
-      <c r="J166" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J166" s="3"/>
       <c r="K166" s="1"/>
       <c r="L166" s="10"/>
       <c r="M166" s="1"/>
@@ -7110,9 +6952,7 @@
       <c r="G167" s="29"/>
       <c r="H167" s="35"/>
       <c r="I167" s="29"/>
-      <c r="J167" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J167" s="3"/>
       <c r="K167" s="1"/>
       <c r="L167" s="10"/>
       <c r="M167" s="1"/>
@@ -7145,9 +6985,7 @@
       <c r="G168" s="29"/>
       <c r="H168" s="35"/>
       <c r="I168" s="29"/>
-      <c r="J168" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J168" s="3"/>
       <c r="K168" s="1"/>
       <c r="L168" s="10"/>
       <c r="M168" s="1"/>
@@ -7180,9 +7018,7 @@
       <c r="G169" s="29"/>
       <c r="H169" s="35"/>
       <c r="I169" s="29"/>
-      <c r="J169" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J169" s="3"/>
       <c r="K169" s="1"/>
       <c r="L169" s="10"/>
       <c r="M169" s="1"/>
@@ -7215,9 +7051,7 @@
       <c r="G170" s="29"/>
       <c r="H170" s="35"/>
       <c r="I170" s="29"/>
-      <c r="J170" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J170" s="3"/>
       <c r="K170" s="1"/>
       <c r="L170" s="24"/>
       <c r="M170" s="1"/>
@@ -7250,9 +7084,7 @@
       <c r="G171" s="29"/>
       <c r="H171" s="35"/>
       <c r="I171" s="29"/>
-      <c r="J171" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J171" s="3"/>
       <c r="K171" s="1"/>
       <c r="L171" s="10"/>
       <c r="M171" s="1"/>
@@ -7285,9 +7117,7 @@
       <c r="G172" s="29"/>
       <c r="H172" s="35"/>
       <c r="I172" s="29"/>
-      <c r="J172" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J172" s="3"/>
       <c r="K172" s="1"/>
       <c r="L172" s="10"/>
       <c r="M172" s="1"/>
@@ -7320,9 +7150,7 @@
       <c r="G173" s="29"/>
       <c r="H173" s="35"/>
       <c r="I173" s="29"/>
-      <c r="J173" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J173" s="3"/>
       <c r="K173" s="1"/>
       <c r="L173" s="10"/>
       <c r="M173" s="1"/>
@@ -7355,9 +7183,7 @@
       <c r="G174" s="29"/>
       <c r="H174" s="29"/>
       <c r="I174" s="29"/>
-      <c r="J174" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J174" s="3"/>
       <c r="K174" s="1"/>
       <c r="L174" s="4"/>
       <c r="M174" s="1"/>
@@ -7390,9 +7216,7 @@
       <c r="G175" s="29"/>
       <c r="H175" s="29"/>
       <c r="I175" s="29"/>
-      <c r="J175" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J175" s="3"/>
       <c r="K175" s="1"/>
       <c r="L175" s="10"/>
       <c r="M175" s="1"/>
@@ -7458,9 +7282,7 @@
       <c r="G177" s="29"/>
       <c r="H177" s="35"/>
       <c r="I177" s="29"/>
-      <c r="J177" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J177" s="3"/>
       <c r="K177" s="1"/>
       <c r="L177" s="10"/>
       <c r="M177" s="1"/>
@@ -7493,9 +7315,7 @@
       <c r="G178" s="29"/>
       <c r="H178" s="35"/>
       <c r="I178" s="29"/>
-      <c r="J178" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J178" s="3"/>
       <c r="K178" s="1"/>
       <c r="L178" s="10"/>
       <c r="M178" s="1"/>
@@ -7561,9 +7381,7 @@
       <c r="G180" s="29"/>
       <c r="H180" s="35"/>
       <c r="I180" s="29"/>
-      <c r="J180" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J180" s="3"/>
       <c r="K180" s="1"/>
       <c r="L180" s="10"/>
       <c r="M180" s="1"/>
@@ -7629,9 +7447,7 @@
       <c r="G182" s="35"/>
       <c r="H182" s="35"/>
       <c r="I182" s="29"/>
-      <c r="J182" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="J182" s="12"/>
       <c r="K182" s="13"/>
       <c r="L182" s="14"/>
       <c r="M182" s="1"/>
@@ -7664,9 +7480,7 @@
       <c r="G183" s="29"/>
       <c r="H183" s="35"/>
       <c r="I183" s="29"/>
-      <c r="J183" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J183" s="3"/>
       <c r="K183" s="1"/>
       <c r="L183" s="10"/>
       <c r="M183" s="1"/>
@@ -7699,9 +7513,7 @@
       <c r="G184" s="29"/>
       <c r="H184" s="35"/>
       <c r="I184" s="29"/>
-      <c r="J184" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J184" s="3"/>
       <c r="K184" s="1"/>
       <c r="L184" s="10"/>
       <c r="M184" s="1"/>
@@ -7734,9 +7546,7 @@
       <c r="G185" s="29"/>
       <c r="H185" s="29"/>
       <c r="I185" s="29"/>
-      <c r="J185" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J185" s="3"/>
       <c r="K185" s="1"/>
       <c r="L185" s="10"/>
       <c r="M185" s="1"/>
@@ -7769,9 +7579,7 @@
       <c r="G186" s="29"/>
       <c r="H186" s="29"/>
       <c r="I186" s="29"/>
-      <c r="J186" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J186" s="3"/>
       <c r="K186" s="1"/>
       <c r="L186" s="10"/>
       <c r="M186" s="1"/>
@@ -7903,9 +7711,7 @@
       <c r="G190" s="29"/>
       <c r="H190" s="35"/>
       <c r="I190" s="29"/>
-      <c r="J190" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J190" s="3"/>
       <c r="K190" s="1"/>
       <c r="L190" s="10"/>
       <c r="M190" s="1"/>
@@ -7971,9 +7777,7 @@
       <c r="G192" s="29"/>
       <c r="H192" s="29"/>
       <c r="I192" s="29"/>
-      <c r="J192" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J192" s="3"/>
       <c r="K192" s="1"/>
       <c r="L192" s="10"/>
       <c r="M192" s="1"/>
@@ -8006,9 +7810,7 @@
       <c r="G193" s="29"/>
       <c r="H193" s="29"/>
       <c r="I193" s="29"/>
-      <c r="J193" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J193" s="3"/>
       <c r="K193" s="1"/>
       <c r="L193" s="10"/>
       <c r="M193" s="1"/>
@@ -8041,9 +7843,7 @@
       <c r="G194" s="29"/>
       <c r="H194" s="29"/>
       <c r="I194" s="29"/>
-      <c r="J194" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J194" s="3"/>
       <c r="K194" s="1"/>
       <c r="L194" s="10"/>
       <c r="M194" s="1"/>
@@ -8076,9 +7876,7 @@
       <c r="G195" s="29"/>
       <c r="H195" s="29"/>
       <c r="I195" s="29"/>
-      <c r="J195" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J195" s="3"/>
       <c r="K195" s="1"/>
       <c r="L195" s="10"/>
       <c r="M195" s="1"/>
@@ -8111,9 +7909,7 @@
       <c r="G196" s="29"/>
       <c r="H196" s="29"/>
       <c r="I196" s="29"/>
-      <c r="J196" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J196" s="3"/>
       <c r="K196" s="1"/>
       <c r="L196" s="10"/>
       <c r="M196" s="1"/>
@@ -8146,9 +7942,7 @@
       <c r="G197" s="29"/>
       <c r="H197" s="29"/>
       <c r="I197" s="29"/>
-      <c r="J197" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="J197" s="3"/>
       <c r="K197" s="1"/>
       <c r="L197" s="10"/>
       <c r="M197" s="1"/>

</xml_diff>